<commit_message>
Phuong - sua lai sprint2 planning, Hung sua lai user-case
</commit_message>
<xml_diff>
--- a/MyTeamWork/Planning/Subsystem.xlsx
+++ b/MyTeamWork/Planning/Subsystem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document Storage\KIEN TAP VTI\MyTeamWork\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0685139-CE6E-4C6A-B7BA-405D6DEB7395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA54505-8ECA-4DCE-85CC-213372257DFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <r>
       <rPr>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -745,6 +748,88 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -757,73 +842,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -833,38 +866,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1206,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -1237,10 +1240,10 @@
       <c r="C1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="21" t="s">
         <v>51</v>
       </c>
@@ -1252,19 +1255,19 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="30"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -1274,19 +1277,19 @@
       <c r="H2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="44"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="34" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="30"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="2">
         <v>1</v>
       </c>
@@ -1304,19 +1307,19 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="31" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="33">
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
@@ -1330,17 +1333,17 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="34" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="13" t="s">
         <v>35</v>
       </c>
@@ -1353,77 +1356,77 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="35" t="s">
+      <c r="A6" s="54"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="33">
         <v>2</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="35" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="39"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="38"/>
       <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="45"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="38" t="s">
+      <c r="A8" s="54"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="41"/>
-      <c r="H8" s="45"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="41"/>
       <c r="K8" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38" t="s">
+      <c r="A9" s="54"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="47"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="36"/>
       <c r="K9" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="31" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="45" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1446,9 +1449,9 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1469,15 +1472,15 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="1">
         <v>2</v>
       </c>
@@ -1489,15 +1492,15 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="1">
         <v>3</v>
       </c>
@@ -1509,50 +1512,50 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="35" t="s">
+      <c r="A14" s="54"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="1">
         <v>2</v>
       </c>
-      <c r="G14" s="40">
-        <v>3</v>
-      </c>
-      <c r="H14" s="33" t="s">
+      <c r="G14" s="33">
+        <v>3</v>
+      </c>
+      <c r="H14" s="35" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38" t="s">
+      <c r="A15" s="54"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="47"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="36"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="15">
         <v>2</v>
       </c>
@@ -1564,81 +1567,81 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64">
-        <v>3</v>
-      </c>
-      <c r="G17" s="65">
-        <v>3</v>
-      </c>
-      <c r="H17" s="61" t="s">
+      <c r="E17" s="49"/>
+      <c r="F17" s="26">
+        <v>3</v>
+      </c>
+      <c r="G17" s="30">
+        <v>3</v>
+      </c>
+      <c r="H17" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59" t="s">
+      <c r="A18" s="59"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="64">
+      <c r="E18" s="32"/>
+      <c r="F18" s="26">
         <v>2</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="H18" s="61"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59" t="s">
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="59"/>
-      <c r="F19" s="64">
-        <v>3</v>
-      </c>
-      <c r="G19" s="65"/>
-      <c r="H19" s="61"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="26">
+        <v>3</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59" t="s">
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="59"/>
-      <c r="F20" s="64">
+      <c r="E20" s="32"/>
+      <c r="F20" s="26">
         <v>2</v>
       </c>
-      <c r="G20" s="65"/>
-      <c r="H20" s="61"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="60" t="s">
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="58"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="14">
         <v>3</v>
       </c>
@@ -1671,6 +1674,27 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="37">
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="G17:G20"/>
@@ -1684,30 +1708,9 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="G6:G9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="B2:B16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="A17:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1725,30 +1728,30 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1762,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD2A12E-971F-4966-A8AD-C05EF522C839}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1788,10 +1791,10 @@
       <c r="C1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="21" t="s">
         <v>51</v>
       </c>
@@ -1803,19 +1806,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="51"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -1823,17 +1826,17 @@
         <v>2</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="34" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="51"/>
+      <c r="E3" s="65"/>
       <c r="F3" s="2">
         <v>1</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="J3" s="22"/>
       <c r="K3" s="24" t="s">
@@ -1849,210 +1852,178 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="31" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="33">
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="34" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="51"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="13" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K5" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="35" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="33">
         <v>2</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>35</v>
+      <c r="H6" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="K6" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="39"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="38"/>
       <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="45"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="38" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="41"/>
-      <c r="H8" s="45"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="47"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="62"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="A11" s="62"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="A12" s="62"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="51"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="47"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-      <c r="B16" s="54"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="13"/>
@@ -2071,6 +2042,21 @@
     <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="B2:B16"/>
     <mergeCell ref="C2:C3"/>
@@ -2082,21 +2068,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="H6:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>